<commit_message>
Streamline project by removing unnecessary files and fixing configurations
Removes unnecessary scripts, fixes DB config, updates web server & screenshot management, and enhances monitoring.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7242c9e3-1c7d-4770-bc2a-a542c4aeed2f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/45399ea3-630c-4463-8e3d-edea73bb30a7/26d18e8b-3001-46e5-a9fd-71c5bab6cbb7.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/missing_draws.xlsx
+++ b/attached_assets/missing_draws.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,54 +451,115 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Winning Numbers (Numerical)</t>
+          <t>Winning Numbers</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Bonus Ball</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PowerBall</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1610</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45776.875</v>
+          <t>Lotto</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-05-01</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7, 16, 19, 20, 39</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>7</v>
+          <t>01, 05, 12, 26, 33, 45</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Daily Lottery</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2237</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45776.75</v>
+          <t>Lotto Plus 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>567</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-05-01</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1, 7, 8, 19, 27</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>07, 14, 21, 28, 35, 42</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PowerBall</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>890</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>03, 11, 22, 33, 44</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>